<commit_message>
added Accounting Equation template
</commit_message>
<xml_diff>
--- a/Documents/Accounting Equation.xlsx
+++ b/Documents/Accounting Equation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydnicholson/Documents/GitHub/accounting-app/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0EA6490-C0F7-8041-88AC-BC5076C90ED1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719BF08B-B342-5F43-8256-47F2210491F4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{FA2973F7-7B77-A140-8E17-44680C9A4F59}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{FA2973F7-7B77-A140-8E17-44680C9A4F59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Account debited</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>NAME:</t>
   </si>
 </sst>
 </file>
@@ -93,9 +96,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -104,11 +105,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,272 +425,299 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17758E6C-C77E-0942-9316-E1170DD1DD70}">
-  <dimension ref="A2:H27"/>
+  <dimension ref="B2:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="224" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:H11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="3.5" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
+        <v>9</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="1">
+        <v>10</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="1">
+        <v>11</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>12</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="1">
+        <v>13</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="1">
+        <v>14</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="1">
+        <v>15</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="1">
+        <v>16</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="1">
+        <v>17</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="1"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="1">
+        <v>18</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="1">
+        <v>19</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>20</v>
+      </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>21</v>
+      </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>22</v>
+      </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="1">
+        <v>23</v>
+      </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="1">
+        <v>24</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <v>25</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>